<commit_message>
updated code for beta 2 migration
</commit_message>
<xml_diff>
--- a/TDG.CORE.ETL.RESOURCES/CLIENT_FILES/TDG_Inspectors.xlsx
+++ b/TDG.CORE.ETL.RESOURCES/CLIENT_FILES/TDG_Inspectors.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3977" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3977" uniqueCount="1421">
   <si>
     <t>(Do Not Modify) Contact</t>
   </si>
@@ -5088,15 +5088,26 @@
   <si>
     <t>Region ID</t>
   </si>
+  <si>
+    <t>National Capital Region</t>
+  </si>
+  <si>
+    <t>Prairie and Northern Region</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -5119,7 +5130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -5129,6 +5140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5493,8 +5505,8 @@
   <sheetPr codeName="dataSheet"/>
   <dimension ref="A1:P205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="K77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N84" sqref="N84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5510,7 +5522,8 @@
     <col min="9" max="9" width="48" style="8" customWidth="1"/>
     <col min="10" max="10" width="59.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29.140625" style="7" customWidth="1"/>
-    <col min="12" max="13" width="17" style="8" customWidth="1"/>
+    <col min="12" max="12" width="17" style="8" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="38.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="42.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="45.140625" style="8" bestFit="1" customWidth="1"/>
@@ -5596,12 +5609,12 @@
       <c r="L2" s="6">
         <v>99901377</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>981</v>
+      <c r="M2" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N2" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O2" s="6" t="s">
         <v>957</v>
@@ -5642,12 +5655,12 @@
       <c r="L3" s="6">
         <v>11110000</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>981</v>
+      <c r="M3" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N3" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O3" s="6" t="s">
         <v>957</v>
@@ -5688,12 +5701,12 @@
       <c r="L4" s="6">
         <v>99901470</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>981</v>
+      <c r="M4" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N4" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O4" s="6" t="s">
         <v>957</v>
@@ -5734,12 +5747,12 @@
       <c r="L5" s="6">
         <v>99900844</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>981</v>
+      <c r="M5" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N5" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O5" s="6" t="s">
         <v>957</v>
@@ -5780,12 +5793,12 @@
       <c r="L6" s="6">
         <v>99900840</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>981</v>
+      <c r="M6" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N6" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O6" s="6" t="s">
         <v>957</v>
@@ -5826,12 +5839,12 @@
       <c r="L7" s="6">
         <v>99901290</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>981</v>
+      <c r="M7" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N7" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O7" s="6" t="s">
         <v>957</v>
@@ -5872,12 +5885,12 @@
       <c r="L8" s="6">
         <v>99900764</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>981</v>
+      <c r="M8" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N8" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O8" s="6" t="s">
         <v>957</v>
@@ -5918,12 +5931,12 @@
       <c r="L9" s="6">
         <v>99900845</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>981</v>
+      <c r="M9" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N9" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O9" s="6" t="s">
         <v>957</v>
@@ -5964,12 +5977,12 @@
       <c r="L10" s="6">
         <v>99901096</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>981</v>
+      <c r="M10" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N10" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O10" s="6" t="s">
         <v>957</v>
@@ -6010,12 +6023,12 @@
       <c r="L11" s="6">
         <v>99900765</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>981</v>
+      <c r="M11" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N11" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O11" s="6" t="s">
         <v>957</v>
@@ -6056,12 +6069,12 @@
       <c r="L12" s="6">
         <v>99901364</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>981</v>
+      <c r="M12" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N12" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O12" s="6" t="s">
         <v>957</v>
@@ -6102,12 +6115,12 @@
       <c r="L13" s="6">
         <v>99901424</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>981</v>
+      <c r="M13" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N13" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O13" s="6" t="s">
         <v>957</v>
@@ -6148,12 +6161,12 @@
       <c r="L14" s="6">
         <v>99901460</v>
       </c>
-      <c r="M14" s="6" t="s">
-        <v>981</v>
+      <c r="M14" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N14" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O14" s="6" t="s">
         <v>957</v>
@@ -6194,12 +6207,12 @@
       <c r="L15" s="6">
         <v>99901425</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>981</v>
+      <c r="M15" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N15" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O15" s="6" t="s">
         <v>957</v>
@@ -6240,12 +6253,12 @@
       <c r="L16" s="6">
         <v>99901537</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>981</v>
+      <c r="M16" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N16" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O16" s="6" t="s">
         <v>957</v>
@@ -6286,12 +6299,12 @@
       <c r="L17" s="6">
         <v>99901382</v>
       </c>
-      <c r="M17" s="6" t="s">
-        <v>981</v>
+      <c r="M17" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N17" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O17" s="6" t="s">
         <v>957</v>
@@ -6332,12 +6345,12 @@
       <c r="L18" s="6">
         <v>99003843</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>981</v>
+      <c r="M18" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N18" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O18" s="6" t="s">
         <v>959</v>
@@ -6378,12 +6391,12 @@
       <c r="L19" s="6">
         <v>111120</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>981</v>
+      <c r="M19" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N19" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O19" s="6" t="s">
         <v>959</v>
@@ -6424,12 +6437,12 @@
       <c r="L20" s="6">
         <v>1111199</v>
       </c>
-      <c r="M20" s="6" t="s">
-        <v>981</v>
+      <c r="M20" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N20" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O20" s="6" t="s">
         <v>959</v>
@@ -6470,12 +6483,12 @@
       <c r="L21" s="6">
         <v>1221212121212120</v>
       </c>
-      <c r="M21" s="6" t="s">
-        <v>981</v>
+      <c r="M21" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N21" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O21" s="6" t="s">
         <v>959</v>
@@ -6516,12 +6529,12 @@
       <c r="L22" s="6">
         <v>99003314</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>981</v>
+      <c r="M22" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N22" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O22" s="6" t="s">
         <v>959</v>
@@ -6562,12 +6575,12 @@
       <c r="L23" s="6">
         <v>99003445</v>
       </c>
-      <c r="M23" s="6" t="s">
-        <v>981</v>
+      <c r="M23" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N23" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O23" s="6" t="s">
         <v>959</v>
@@ -6608,12 +6621,12 @@
       <c r="L24" s="6">
         <v>99003446</v>
       </c>
-      <c r="M24" s="6" t="s">
-        <v>981</v>
+      <c r="M24" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N24" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O24" s="6" t="s">
         <v>959</v>
@@ -6654,12 +6667,12 @@
       <c r="L25" s="6">
         <v>99003560</v>
       </c>
-      <c r="M25" s="6" t="s">
-        <v>981</v>
+      <c r="M25" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N25" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O25" s="6" t="s">
         <v>959</v>
@@ -6700,12 +6713,12 @@
       <c r="L26" s="6">
         <v>12345667</v>
       </c>
-      <c r="M26" s="6" t="s">
-        <v>981</v>
+      <c r="M26" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N26" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O26" s="6" t="s">
         <v>959</v>
@@ -6746,12 +6759,12 @@
       <c r="L27" s="6">
         <v>99003326</v>
       </c>
-      <c r="M27" s="6" t="s">
-        <v>981</v>
+      <c r="M27" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N27" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O27" s="6" t="s">
         <v>959</v>
@@ -6792,12 +6805,12 @@
       <c r="L28" s="6">
         <v>99003307</v>
       </c>
-      <c r="M28" s="6" t="s">
-        <v>981</v>
+      <c r="M28" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N28" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O28" s="6" t="s">
         <v>959</v>
@@ -6838,12 +6851,12 @@
       <c r="L29" s="6">
         <v>9003255</v>
       </c>
-      <c r="M29" s="6" t="s">
-        <v>981</v>
+      <c r="M29" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N29" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O29" s="6" t="s">
         <v>959</v>
@@ -6884,12 +6897,12 @@
       <c r="L30" s="6">
         <v>99003688</v>
       </c>
-      <c r="M30" s="6" t="s">
-        <v>981</v>
+      <c r="M30" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N30" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O30" s="6" t="s">
         <v>959</v>
@@ -6930,12 +6943,12 @@
       <c r="L31" s="6">
         <v>99901284</v>
       </c>
-      <c r="M31" s="6" t="s">
-        <v>981</v>
+      <c r="M31" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N31" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O31" s="6" t="s">
         <v>959</v>
@@ -6976,12 +6989,12 @@
       <c r="L32" s="6">
         <v>99901328</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>981</v>
+      <c r="M32" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N32" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O32" s="6" t="s">
         <v>959</v>
@@ -7022,12 +7035,12 @@
       <c r="L33" s="6">
         <v>99003447</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>981</v>
+      <c r="M33" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N33" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O33" s="6" t="s">
         <v>959</v>
@@ -7068,12 +7081,12 @@
       <c r="L34" s="6">
         <v>99003550</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>981</v>
+      <c r="M34" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N34" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O34" s="6" t="s">
         <v>959</v>
@@ -7114,12 +7127,12 @@
       <c r="L35" s="6">
         <v>99900422</v>
       </c>
-      <c r="M35" s="6" t="s">
-        <v>981</v>
+      <c r="M35" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N35" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O35" s="6" t="s">
         <v>959</v>
@@ -7160,12 +7173,12 @@
       <c r="L36" s="6">
         <v>101010101</v>
       </c>
-      <c r="M36" s="6" t="s">
-        <v>981</v>
+      <c r="M36" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N36" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O36" s="6" t="s">
         <v>961</v>
@@ -7206,12 +7219,12 @@
       <c r="L37" s="6">
         <v>3111111</v>
       </c>
-      <c r="M37" s="6" t="s">
-        <v>981</v>
+      <c r="M37" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N37" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O37" s="6" t="s">
         <v>961</v>
@@ -7252,12 +7265,12 @@
       <c r="L38" s="6">
         <v>222222222222222</v>
       </c>
-      <c r="M38" s="6" t="s">
-        <v>981</v>
+      <c r="M38" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N38" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O38" s="6" t="s">
         <v>961</v>
@@ -7298,12 +7311,12 @@
       <c r="L39" s="6">
         <v>55555555</v>
       </c>
-      <c r="M39" s="6" t="s">
-        <v>981</v>
+      <c r="M39" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N39" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O39" s="6" t="s">
         <v>961</v>
@@ -7344,12 +7357,12 @@
       <c r="L40" s="6">
         <v>0</v>
       </c>
-      <c r="M40" s="6" t="s">
-        <v>981</v>
+      <c r="M40" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N40" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O40" s="6" t="s">
         <v>961</v>
@@ -7390,12 +7403,12 @@
       <c r="L41" s="6">
         <v>111111113</v>
       </c>
-      <c r="M41" s="6" t="s">
-        <v>981</v>
+      <c r="M41" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N41" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O41" s="6" t="s">
         <v>961</v>
@@ -7436,12 +7449,12 @@
       <c r="L42" s="6">
         <v>1111111122</v>
       </c>
-      <c r="M42" s="6" t="s">
-        <v>981</v>
+      <c r="M42" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N42" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O42" s="6" t="s">
         <v>961</v>
@@ -7482,12 +7495,12 @@
       <c r="L43" s="6">
         <v>1111122</v>
       </c>
-      <c r="M43" s="6" t="s">
-        <v>981</v>
+      <c r="M43" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N43" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O43" s="6" t="s">
         <v>961</v>
@@ -7528,12 +7541,12 @@
       <c r="L44" s="6">
         <v>1111111111</v>
       </c>
-      <c r="M44" s="6" t="s">
-        <v>981</v>
+      <c r="M44" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N44" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O44" s="6" t="s">
         <v>961</v>
@@ -7574,12 +7587,12 @@
       <c r="L45" s="6">
         <v>99901366</v>
       </c>
-      <c r="M45" s="6" t="s">
-        <v>981</v>
+      <c r="M45" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N45" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O45" s="6" t="s">
         <v>961</v>
@@ -7615,12 +7628,12 @@
       <c r="L46" s="6">
         <v>123456</v>
       </c>
-      <c r="M46" s="6" t="s">
-        <v>981</v>
+      <c r="M46" s="9" t="s">
+        <v>1419</v>
       </c>
       <c r="N46" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>04b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O46" s="6" t="s">
         <v>961</v>
@@ -7661,12 +7674,12 @@
       <c r="L47" s="6">
         <v>922922</v>
       </c>
-      <c r="M47" s="6" t="s">
-        <v>982</v>
+      <c r="M47" t="s">
+        <v>1420</v>
       </c>
       <c r="N47" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O47" s="6" t="s">
         <v>963</v>
@@ -7707,12 +7720,12 @@
       <c r="L48" s="6">
         <v>911911</v>
       </c>
-      <c r="M48" s="6" t="s">
-        <v>982</v>
+      <c r="M48" t="s">
+        <v>1420</v>
       </c>
       <c r="N48" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O48" s="6" t="s">
         <v>963</v>
@@ -7753,12 +7766,12 @@
       <c r="L49" s="6">
         <v>989898</v>
       </c>
-      <c r="M49" s="6" t="s">
-        <v>982</v>
+      <c r="M49" t="s">
+        <v>1420</v>
       </c>
       <c r="N49" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O49" s="6" t="s">
         <v>963</v>
@@ -7799,12 +7812,12 @@
       <c r="L50" s="6">
         <v>979797</v>
       </c>
-      <c r="M50" s="6" t="s">
-        <v>982</v>
+      <c r="M50" t="s">
+        <v>1420</v>
       </c>
       <c r="N50" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O50" s="6" t="s">
         <v>963</v>
@@ -7845,12 +7858,12 @@
       <c r="L51" s="6">
         <v>969696</v>
       </c>
-      <c r="M51" s="6" t="s">
-        <v>982</v>
+      <c r="M51" t="s">
+        <v>1420</v>
       </c>
       <c r="N51" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O51" s="6" t="s">
         <v>963</v>
@@ -7891,12 +7904,12 @@
       <c r="L52" s="6">
         <v>99003684</v>
       </c>
-      <c r="M52" s="6" t="s">
-        <v>982</v>
+      <c r="M52" t="s">
+        <v>1420</v>
       </c>
       <c r="N52" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O52" s="6" t="s">
         <v>963</v>
@@ -7937,12 +7950,12 @@
       <c r="L53" s="6">
         <v>99003465</v>
       </c>
-      <c r="M53" s="6" t="s">
-        <v>982</v>
+      <c r="M53" t="s">
+        <v>1420</v>
       </c>
       <c r="N53" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O53" s="6" t="s">
         <v>963</v>
@@ -7978,12 +7991,12 @@
       <c r="L54" s="6">
         <v>99003486</v>
       </c>
-      <c r="M54" s="6" t="s">
-        <v>982</v>
+      <c r="M54" t="s">
+        <v>1420</v>
       </c>
       <c r="N54" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O54" s="6" t="s">
         <v>963</v>
@@ -8024,12 +8037,12 @@
       <c r="L55" s="6">
         <v>11111112</v>
       </c>
-      <c r="M55" s="6" t="s">
-        <v>982</v>
+      <c r="M55" t="s">
+        <v>1420</v>
       </c>
       <c r="N55" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O55" s="6" t="s">
         <v>963</v>
@@ -8065,12 +8078,12 @@
       <c r="L56" s="6">
         <v>999999999</v>
       </c>
-      <c r="M56" s="6" t="s">
-        <v>982</v>
+      <c r="M56" t="s">
+        <v>1420</v>
       </c>
       <c r="N56" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O56" s="6" t="s">
         <v>963</v>
@@ -8111,12 +8124,12 @@
       <c r="L57" s="6">
         <v>99003471</v>
       </c>
-      <c r="M57" s="6" t="s">
-        <v>982</v>
+      <c r="M57" t="s">
+        <v>1420</v>
       </c>
       <c r="N57" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O57" s="6" t="s">
         <v>963</v>
@@ -8157,12 +8170,12 @@
       <c r="L58" s="6">
         <v>99002758</v>
       </c>
-      <c r="M58" s="6" t="s">
-        <v>982</v>
+      <c r="M58" t="s">
+        <v>1420</v>
       </c>
       <c r="N58" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O58" s="6" t="s">
         <v>963</v>
@@ -8203,12 +8216,12 @@
       <c r="L59" s="6">
         <v>99002757</v>
       </c>
-      <c r="M59" s="6" t="s">
-        <v>982</v>
+      <c r="M59" t="s">
+        <v>1420</v>
       </c>
       <c r="N59" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O59" s="6" t="s">
         <v>963</v>
@@ -8249,12 +8262,12 @@
       <c r="L60" s="6">
         <v>99002614</v>
       </c>
-      <c r="M60" s="6" t="s">
-        <v>982</v>
+      <c r="M60" t="s">
+        <v>1420</v>
       </c>
       <c r="N60" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O60" s="6" t="s">
         <v>963</v>
@@ -8295,12 +8308,12 @@
       <c r="L61" s="6">
         <v>99002615</v>
       </c>
-      <c r="M61" s="6" t="s">
-        <v>982</v>
+      <c r="M61" t="s">
+        <v>1420</v>
       </c>
       <c r="N61" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O61" s="6" t="s">
         <v>963</v>
@@ -8341,12 +8354,12 @@
       <c r="L62" s="6">
         <v>99002616</v>
       </c>
-      <c r="M62" s="6" t="s">
-        <v>982</v>
+      <c r="M62" t="s">
+        <v>1420</v>
       </c>
       <c r="N62" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O62" s="6" t="s">
         <v>963</v>
@@ -8387,12 +8400,12 @@
       <c r="L63" s="6">
         <v>0</v>
       </c>
-      <c r="M63" s="6" t="s">
-        <v>982</v>
+      <c r="M63" t="s">
+        <v>1420</v>
       </c>
       <c r="N63" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O63" s="6" t="s">
         <v>963</v>
@@ -8433,12 +8446,12 @@
       <c r="L64" s="6">
         <v>99901210</v>
       </c>
-      <c r="M64" s="6" t="s">
-        <v>982</v>
+      <c r="M64" t="s">
+        <v>1420</v>
       </c>
       <c r="N64" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O64" s="6" t="s">
         <v>963</v>
@@ -8479,12 +8492,12 @@
       <c r="L65" s="6">
         <v>99003466</v>
       </c>
-      <c r="M65" s="6" t="s">
-        <v>982</v>
+      <c r="M65" t="s">
+        <v>1420</v>
       </c>
       <c r="N65" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O65" s="6" t="s">
         <v>963</v>
@@ -8525,12 +8538,12 @@
       <c r="L66" s="6">
         <v>99003467</v>
       </c>
-      <c r="M66" s="6" t="s">
-        <v>982</v>
+      <c r="M66" t="s">
+        <v>1420</v>
       </c>
       <c r="N66" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O66" s="6" t="s">
         <v>963</v>
@@ -8571,12 +8584,12 @@
       <c r="L67" s="6">
         <v>99003477</v>
       </c>
-      <c r="M67" s="6" t="s">
-        <v>982</v>
+      <c r="M67" t="s">
+        <v>1420</v>
       </c>
       <c r="N67" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O67" s="6" t="s">
         <v>963</v>
@@ -8617,12 +8630,12 @@
       <c r="L68" s="6">
         <v>99002532</v>
       </c>
-      <c r="M68" s="6" t="s">
-        <v>982</v>
+      <c r="M68" t="s">
+        <v>1420</v>
       </c>
       <c r="N68" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O68" s="6" t="s">
         <v>963</v>
@@ -8663,12 +8676,12 @@
       <c r="L69" s="6">
         <v>99002130</v>
       </c>
-      <c r="M69" s="6" t="s">
-        <v>982</v>
+      <c r="M69" t="s">
+        <v>1420</v>
       </c>
       <c r="N69" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O69" s="6" t="s">
         <v>963</v>
@@ -8709,12 +8722,12 @@
       <c r="L70" s="6">
         <v>99002560</v>
       </c>
-      <c r="M70" s="6" t="s">
-        <v>982</v>
+      <c r="M70" t="s">
+        <v>1420</v>
       </c>
       <c r="N70" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O70" s="6" t="s">
         <v>963</v>
@@ -8755,12 +8768,12 @@
       <c r="L71" s="6">
         <v>99003483</v>
       </c>
-      <c r="M71" s="6" t="s">
-        <v>982</v>
+      <c r="M71" t="s">
+        <v>1420</v>
       </c>
       <c r="N71" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O71" s="6" t="s">
         <v>963</v>
@@ -8801,12 +8814,12 @@
       <c r="L72" s="6">
         <v>99003476</v>
       </c>
-      <c r="M72" s="6" t="s">
-        <v>982</v>
+      <c r="M72" t="s">
+        <v>1420</v>
       </c>
       <c r="N72" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O72" s="6" t="s">
         <v>963</v>
@@ -8847,12 +8860,12 @@
       <c r="L73" s="6">
         <v>99900582</v>
       </c>
-      <c r="M73" s="6" t="s">
-        <v>982</v>
+      <c r="M73" t="s">
+        <v>1420</v>
       </c>
       <c r="N73" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O73" s="6" t="s">
         <v>963</v>
@@ -8893,12 +8906,12 @@
       <c r="L74" s="6">
         <v>4</v>
       </c>
-      <c r="M74" s="6" t="s">
-        <v>982</v>
+      <c r="M74" t="s">
+        <v>1420</v>
       </c>
       <c r="N74" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O74" s="6" t="s">
         <v>963</v>
@@ -8939,12 +8952,12 @@
       <c r="L75" s="6">
         <v>99900039</v>
       </c>
-      <c r="M75" s="6" t="s">
-        <v>982</v>
+      <c r="M75" t="s">
+        <v>1420</v>
       </c>
       <c r="N75" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O75" s="6" t="s">
         <v>963</v>
@@ -8985,12 +8998,12 @@
       <c r="L76" s="6">
         <v>99901062</v>
       </c>
-      <c r="M76" s="6" t="s">
-        <v>982</v>
+      <c r="M76" t="s">
+        <v>1420</v>
       </c>
       <c r="N76" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O76" s="6" t="s">
         <v>963</v>
@@ -9031,12 +9044,12 @@
       <c r="L77" s="6">
         <v>99003723</v>
       </c>
-      <c r="M77" s="6" t="s">
-        <v>982</v>
+      <c r="M77" t="s">
+        <v>1420</v>
       </c>
       <c r="N77" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O77" s="6" t="s">
         <v>963</v>
@@ -9077,12 +9090,12 @@
       <c r="L78" s="6">
         <v>99900589</v>
       </c>
-      <c r="M78" s="6" t="s">
-        <v>982</v>
+      <c r="M78" t="s">
+        <v>1420</v>
       </c>
       <c r="N78" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O78" s="6" t="s">
         <v>963</v>
@@ -9123,12 +9136,12 @@
       <c r="L79" s="6">
         <v>99901133</v>
       </c>
-      <c r="M79" s="6" t="s">
-        <v>982</v>
+      <c r="M79" t="s">
+        <v>1420</v>
       </c>
       <c r="N79" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O79" s="6" t="s">
         <v>963</v>
@@ -9169,12 +9182,12 @@
       <c r="L80" s="6">
         <v>99900579</v>
       </c>
-      <c r="M80" s="6" t="s">
-        <v>982</v>
+      <c r="M80" t="s">
+        <v>1420</v>
       </c>
       <c r="N80" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O80" s="6" t="s">
         <v>963</v>
@@ -9215,12 +9228,12 @@
       <c r="L81" s="6">
         <v>99900690</v>
       </c>
-      <c r="M81" s="6" t="s">
-        <v>982</v>
+      <c r="M81" t="s">
+        <v>1420</v>
       </c>
       <c r="N81" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O81" s="6" t="s">
         <v>963</v>
@@ -9261,12 +9274,12 @@
       <c r="L82" s="6">
         <v>0</v>
       </c>
-      <c r="M82" s="6" t="s">
-        <v>982</v>
+      <c r="M82" t="s">
+        <v>1420</v>
       </c>
       <c r="N82" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O82" s="6" t="s">
         <v>963</v>
@@ -9307,12 +9320,12 @@
       <c r="L83" s="6">
         <v>1</v>
       </c>
-      <c r="M83" s="6" t="s">
-        <v>982</v>
+      <c r="M83" t="s">
+        <v>1420</v>
       </c>
       <c r="N83" s="6" t="str">
         <f>IF(Table1[[#This Row],[Region]]="NCR", "04b86e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="ONT", "50b21a84-db04-eb11-a813-000d3af3ac0d", IF(Table1[[#This Row],[Region]]="ATL", "fab76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PQ", "fcb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PAC", "feb76e9e-1707-eb11-a813-000d3af3a0d7", IF(Table1[[#This Row],[Region]]="PNR", "02b86e9e-1707-eb11-a813-000d3af3a0d7", ""))))))</f>
-        <v>02b86e9e-1707-eb11-a813-000d3af3a0d7</v>
+        <v/>
       </c>
       <c r="O83" s="6" t="s">
         <v>963</v>
@@ -14804,7 +14817,7 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 50 characters long." promptTitle="Text (required)" prompt="Maximum Length: 50 characters." sqref="E205:E1048576 F204:I1048576">
       <formula1>50</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 50 characters long." promptTitle="Text" prompt="Maximum Length: 50 characters." sqref="E2:E203 P2:P1048576 K2:K1048576 L2:O203">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 50 characters long." promptTitle="Text" prompt="Maximum Length: 50 characters." sqref="E2:E203 P2:P1048576 K2:K1048576 L2:L203 N2:O203 M2:M46 M84:M203">
       <formula1>50</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 160 characters long." promptTitle="Text" prompt="Maximum Length: 160 characters." sqref="F2:H203">
@@ -14818,8 +14831,9 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>